<commit_message>
Zero value now have a white color as default. Value to 48 hour now have gray color.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Программирование\Проекты\visitka_count\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr showInkAnnotation="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Лист3" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
@@ -96,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,7 +139,7 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -162,6 +157,21 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color indexed="23"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color indexed="23"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,9 +190,188 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -198,37 +387,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="dashDot">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -237,170 +400,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDot">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDot">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="dashDot">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDot">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -409,41 +419,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -452,89 +462,92 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -581,7 +594,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -616,7 +629,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,42 +806,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="42"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="27" customHeight="1">
+      <c r="A1" s="25"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="46"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A2" s="5">
         <v>250</v>
       </c>
@@ -848,136 +860,136 @@
         <v>0</v>
       </c>
       <c r="I2" s="38"/>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="40"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="38" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="38"/>
       <c r="N2" s="17"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="12">
         <v>500</v>
       </c>
       <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="25"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="23"/>
-      <c r="G3" s="25"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="23"/>
-      <c r="I3" s="25"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="25"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="23"/>
-      <c r="M3" s="26"/>
-    </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="33"/>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A4" s="13">
         <v>1000</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="29"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="34"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="27">
         <f>FLOOR(SUM(B3:B4), 1)</f>
         <v>0</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="31">
         <f>FLOOR(SUM(C3:C4), 1)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="28">
         <f t="shared" ref="D5:M5" si="0">FLOOR(SUM(D3:D4), 1)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="45">
+      <c r="J5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="45">
+      <c r="K5" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="33"/>
+    <row r="6" spans="1:18" ht="27" customHeight="1">
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="40"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="33"/>
-    </row>
-    <row r="8" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="27" customHeight="1">
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="40"/>
+    </row>
+    <row r="8" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A8" s="5">
         <v>300</v>
       </c>
@@ -997,133 +1009,133 @@
         <v>3</v>
       </c>
       <c r="I8" s="38"/>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="40"/>
+      <c r="K8" s="44"/>
       <c r="L8" s="38" t="s">
         <v>15</v>
       </c>
       <c r="M8" s="38"/>
     </row>
-    <row r="9" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="27" customHeight="1">
       <c r="A9" s="12">
         <v>500</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="25"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="25"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="23"/>
-      <c r="I9" s="25"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="23"/>
-      <c r="K9" s="25"/>
+      <c r="K9" s="32"/>
       <c r="L9" s="23"/>
-      <c r="M9" s="26"/>
-    </row>
-    <row r="10" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M9" s="33"/>
+    </row>
+    <row r="10" spans="1:18" ht="27" customHeight="1">
       <c r="A10" s="13">
         <v>1000</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="29"/>
-    </row>
-    <row r="11" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="24"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="28">
         <f t="shared" ref="B11:M11" si="1">FLOOR(SUM(B9:B10), 1)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="45">
+      <c r="H11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="45">
+      <c r="I11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="45">
+      <c r="J11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L11" s="45">
+      <c r="L11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M11" s="45">
+      <c r="M11" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="33"/>
-    </row>
-    <row r="13" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="33"/>
-    </row>
-    <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="27" customHeight="1">
+      <c r="A12" s="43"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="40"/>
+    </row>
+    <row r="13" spans="1:18" ht="27" customHeight="1">
+      <c r="A13" s="43"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="40"/>
+    </row>
+    <row r="14" spans="1:18" ht="27" customHeight="1">
       <c r="A14" s="5">
         <v>350</v>
       </c>
@@ -1143,150 +1155,150 @@
         <v>5</v>
       </c>
       <c r="I14" s="38"/>
-      <c r="J14" s="40" t="s">
+      <c r="J14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="40"/>
+      <c r="K14" s="44"/>
       <c r="L14" s="38" t="s">
         <v>16</v>
       </c>
       <c r="M14" s="38"/>
     </row>
-    <row r="15" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="27" customHeight="1">
       <c r="A15" s="12">
         <v>500</v>
       </c>
       <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="23"/>
-      <c r="E15" s="25"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="25"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="23"/>
-      <c r="I15" s="25"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="23"/>
-      <c r="K15" s="25"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="23"/>
-      <c r="M15" s="26"/>
-    </row>
-    <row r="16" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="33"/>
+    </row>
+    <row r="16" spans="1:18" ht="27" customHeight="1">
       <c r="A16" s="13">
         <v>1000</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="29"/>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="24"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="34"/>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="28">
         <f t="shared" ref="B17:M17" si="2">FLOOR(SUM(B15:B16), 1)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H17" s="45">
+      <c r="H17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I17" s="45">
+      <c r="I17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="45">
+      <c r="J17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K17" s="45">
+      <c r="K17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="33"/>
-    </row>
-    <row r="19" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="33"/>
-    </row>
-    <row r="20" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="27" customHeight="1">
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="40"/>
+    </row>
+    <row r="19" spans="1:13" ht="27" customHeight="1">
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="40"/>
+    </row>
+    <row r="20" spans="1:13" ht="27" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="33"/>
-    </row>
-    <row r="21" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="41"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="40"/>
+    </row>
+    <row r="21" spans="1:13" ht="27" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="18" t="s">
         <v>8</v>
@@ -1325,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="27" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="9"/>
       <c r="C22" s="2"/>
@@ -1340,7 +1352,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="27" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="9"/>
       <c r="C23" s="2"/>
@@ -1355,7 +1367,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="27" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="9"/>
       <c r="C24" s="2"/>
@@ -1370,7 +1382,7 @@
       <c r="L24" s="9"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="27" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="9"/>
       <c r="C25" s="2"/>
@@ -1385,7 +1397,7 @@
       <c r="L25" s="9"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="27" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="9"/>
       <c r="C26" s="2"/>
@@ -1400,7 +1412,7 @@
       <c r="L26" s="9"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="27" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" s="9"/>
       <c r="C27" s="2"/>
@@ -1415,7 +1427,7 @@
       <c r="L27" s="9"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="27" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="2"/>
@@ -1430,7 +1442,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="27" customHeight="1">
       <c r="A29" s="14" t="s">
         <v>2</v>
       </c>
@@ -1447,7 +1459,7 @@
       <c r="L29" s="9"/>
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="11" t="s">
         <v>7</v>
       </c>
@@ -1466,190 +1478,268 @@
       <c r="L30" s="36"/>
       <c r="M30" s="37"/>
     </row>
-    <row r="31" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="27" customHeight="1">
       <c r="A31" s="4"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-    </row>
-    <row r="32" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+    </row>
+    <row r="32" spans="1:13" ht="27" customHeight="1">
       <c r="A32" s="4"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-    </row>
-    <row r="33" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+    </row>
+    <row r="33" spans="1:13" ht="27" customHeight="1">
       <c r="A33" s="4"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-    </row>
-    <row r="34" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+    </row>
+    <row r="34" spans="1:13" ht="27" customHeight="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-    </row>
-    <row r="35" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+    </row>
+    <row r="35" spans="1:13" ht="27" customHeight="1">
       <c r="A35" s="4"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-    </row>
-    <row r="39" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+    </row>
+    <row r="39" spans="1:13" ht="27" customHeight="1">
       <c r="A39" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="22.5" customHeight="1">
       <c r="A40" s="21"/>
     </row>
-    <row r="41" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="22.5" customHeight="1">
       <c r="A41" s="21"/>
     </row>
-    <row r="42" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="22.5" customHeight="1">
       <c r="A42" s="21"/>
     </row>
-    <row r="43" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="22.5" customHeight="1">
       <c r="A43" s="21"/>
     </row>
-    <row r="44" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="22.5" customHeight="1">
       <c r="A44" s="21"/>
     </row>
-    <row r="45" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="22.5" customHeight="1">
       <c r="A45" s="21"/>
     </row>
-    <row r="46" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="22.5" customHeight="1">
       <c r="A46" s="21"/>
     </row>
-    <row r="47" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="22.5" customHeight="1">
       <c r="A47" s="21"/>
     </row>
-    <row r="48" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="22.5" customHeight="1">
       <c r="A48" s="21"/>
     </row>
-    <row r="49" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="22.5" customHeight="1">
       <c r="A49" s="21"/>
     </row>
-    <row r="50" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="22.5" customHeight="1">
       <c r="A50" s="21"/>
     </row>
-    <row r="51" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" ht="22.5" customHeight="1">
       <c r="A51" s="21"/>
     </row>
-    <row r="52" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" ht="22.5" customHeight="1">
       <c r="A52" s="21"/>
     </row>
-    <row r="53" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" ht="22.5" customHeight="1">
       <c r="A53" s="21"/>
     </row>
-    <row r="54" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" ht="22.5" customHeight="1">
       <c r="A54" s="21"/>
     </row>
-    <row r="55" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" ht="22.5" customHeight="1">
       <c r="A55" s="21"/>
     </row>
-    <row r="56" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" ht="22.5" customHeight="1">
       <c r="A56" s="21"/>
     </row>
-    <row r="57" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" ht="22.5" customHeight="1">
       <c r="A57" s="21"/>
     </row>
-    <row r="58" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" ht="22.5" customHeight="1">
       <c r="A58" s="21"/>
     </row>
-    <row r="59" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" ht="22.5" customHeight="1">
       <c r="A59" s="21"/>
     </row>
-    <row r="60" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="22.5" customHeight="1">
       <c r="A60" s="21"/>
     </row>
-    <row r="61" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" ht="22.5" customHeight="1">
       <c r="A61" s="21"/>
     </row>
-    <row r="62" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" ht="22.5" customHeight="1">
       <c r="A62" s="21"/>
     </row>
-    <row r="63" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" ht="22.5" customHeight="1">
       <c r="A63" s="21"/>
     </row>
-    <row r="64" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" ht="22.5" customHeight="1">
       <c r="A64" s="21"/>
     </row>
-    <row r="65" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" ht="22.5" customHeight="1">
       <c r="A65" s="21"/>
     </row>
-    <row r="66" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" ht="22.5" customHeight="1">
       <c r="A66" s="21"/>
     </row>
-    <row r="67" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" ht="22.5" customHeight="1">
       <c r="A67" s="21"/>
     </row>
-    <row r="68" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" ht="22.5" customHeight="1">
       <c r="A68" s="21"/>
     </row>
-    <row r="69" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" ht="22.5" customHeight="1">
       <c r="A69" s="21"/>
     </row>
-    <row r="70" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" ht="22.5" customHeight="1">
       <c r="A70" s="21"/>
     </row>
-    <row r="71" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" ht="22.5" customHeight="1">
       <c r="A71" s="21"/>
     </row>
-    <row r="72" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" ht="22.5" customHeight="1">
       <c r="A72" s="21"/>
     </row>
-    <row r="73" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" ht="22.5" customHeight="1">
       <c r="A73" s="21"/>
     </row>
-    <row r="74" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" ht="22.5" customHeight="1">
       <c r="A74" s="21"/>
+    </row>
+    <row r="75" spans="1:1" ht="18.75">
+      <c r="A75" s="21"/>
+    </row>
+    <row r="76" spans="1:1" ht="18.75">
+      <c r="A76" s="21"/>
+    </row>
+    <row r="77" spans="1:1" ht="18.75">
+      <c r="A77" s="21"/>
+    </row>
+    <row r="78" spans="1:1" ht="18.75">
+      <c r="A78" s="21"/>
+    </row>
+    <row r="79" spans="1:1" ht="18.75">
+      <c r="A79" s="21"/>
+    </row>
+    <row r="80" spans="1:1" ht="18.75">
+      <c r="A80" s="21"/>
+    </row>
+    <row r="81" spans="1:1" ht="18.75">
+      <c r="A81" s="21"/>
+    </row>
+    <row r="82" spans="1:1" ht="18.75">
+      <c r="A82" s="21"/>
+    </row>
+    <row r="83" spans="1:1" ht="18.75">
+      <c r="A83" s="21"/>
+    </row>
+    <row r="84" spans="1:1" ht="18.75">
+      <c r="A84" s="21"/>
+    </row>
+    <row r="85" spans="1:1" ht="18.75">
+      <c r="A85" s="21"/>
+    </row>
+    <row r="86" spans="1:1" ht="18.75">
+      <c r="A86" s="21"/>
+    </row>
+    <row r="87" spans="1:1" ht="18.75">
+      <c r="A87" s="21"/>
+    </row>
+    <row r="88" spans="1:1" ht="18.75">
+      <c r="A88" s="21"/>
+    </row>
+    <row r="89" spans="1:1" ht="18.75">
+      <c r="A89" s="21"/>
+    </row>
+    <row r="90" spans="1:1" ht="18.75">
+      <c r="A90" s="21"/>
+    </row>
+    <row r="91" spans="1:1" ht="18.75">
+      <c r="A91" s="21"/>
+    </row>
+    <row r="92" spans="1:1" ht="18.75">
+      <c r="A92" s="21"/>
+    </row>
+    <row r="93" spans="1:1" ht="18.75">
+      <c r="A93" s="21"/>
+    </row>
+    <row r="94" spans="1:1" ht="18.75">
+      <c r="A94" s="21"/>
+    </row>
+    <row r="95" spans="1:1" ht="18.75">
+      <c r="A95" s="21"/>
+    </row>
+    <row r="96" spans="1:1" ht="18.75">
+      <c r="A96" s="21"/>
+    </row>
+    <row r="97" spans="1:1" ht="18.75">
+      <c r="A97" s="21"/>
+    </row>
+    <row r="98" spans="1:1" ht="18.75">
+      <c r="A98" s="21"/>
+    </row>
+    <row r="99" spans="1:1" ht="18.75">
+      <c r="A99" s="21"/>
+    </row>
+    <row r="100" spans="1:1" ht="18.75">
+      <c r="A100" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="62">
@@ -1684,7 +1774,6 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B30:M30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
@@ -1695,13 +1784,13 @@
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H33:I33"/>
@@ -1710,13 +1799,19 @@
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="J34:K34"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="L33:M33"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="L35:M35"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
+  <conditionalFormatting sqref="B5:M5 B11:M11 B17:M17">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.98425196850393704" header="0" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>